<commit_message>
Some minor script and records updates
</commit_message>
<xml_diff>
--- a/Records/Cps_locations_updated_Apr2021.xlsx
+++ b/Records/Cps_locations_updated_Apr2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barkebri\Documents\Species\BOXB\Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4CD38A-87E4-475C-A9ED-C36DD3A50447}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F558674F-6748-4F44-A752-853A75EA3ED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1430,15 +1430,6 @@
   </si>
   <si>
     <t>Center for Environmental and Research Information Systems (CERIS). Purdue University. "Survey Status of Boxwood blight; Leaf and stem blight - Calonectria pseudonaviculata  (2020)." Retrieved from http://pest.ceris.purdue.edu/map.php?code=FBBJCXR&amp;year=2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Department of Agriculture Agricultural Research Service Fungal Database, Record No. BPI 892401. Available at: https://nt.ars-grin.gov/fungaldatabases/ </t>
-  </si>
-  <si>
-    <t>US Department of Agriculture Agricultural Research Service Fungal Database, Record No. BPI 893195. Available at: https://nt.ars-grin.gov/fungaldatabases/</t>
-  </si>
-  <si>
-    <t>US Department of Agriculture Agricultural Research Service Fungal Database, Record No. BPI 892392. Available at: https://nt.ars-grin.gov/fungaldatabases/</t>
   </si>
   <si>
     <t>Blomquist CL, Kosta KL, Santos PF, Rooney-Latham S (2018) First report of boxwood blight caused by Calonectria pseudonaviculata in California. Plant Disease 102: 2379–2379. https://doi.org/10.1094/PDIS-05-18-0765-PDN</t>
@@ -1888,6 +1879,15 @@
   </si>
   <si>
     <t>Thesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farr, D.F., &amp; Rossman, A.Y. Fungal Databases, U.S. National Fungus Collections, ARS, USDA. Record No. BPI 892401. Retrieved October 13, 2021, from https://nt.ars-grin.gov/fungaldatabases/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farr, D.F., &amp; Rossman, A.Y. Fungal Databases, U.S. National Fungus Collections, ARS, USDA. Record No. BPI 893195. Retrieved October 13, 2021, from https://nt.ars-grin.gov/fungaldatabases/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farr, D.F., &amp; Rossman, A.Y. Fungal Databases, U.S. National Fungus Collections, ARS, USDA. Record No. BPI 892392. Retrieved October 13, 2021, from https://nt.ars-grin.gov/fungaldatabases/ </t>
   </si>
 </sst>
 </file>
@@ -2258,8 +2258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I297" sqref="I297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3451,7 +3451,7 @@
         <v>2011</v>
       </c>
       <c r="I29" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J29" t="s">
         <v>14</v>
@@ -3495,7 +3495,7 @@
         <v>2012</v>
       </c>
       <c r="I30" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J30" t="s">
         <v>14</v>
@@ -3539,7 +3539,7 @@
         <v>2011</v>
       </c>
       <c r="I31" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J31" t="s">
         <v>14</v>
@@ -3580,7 +3580,7 @@
         <v>2011</v>
       </c>
       <c r="I32" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J32" t="s">
         <v>14</v>
@@ -3665,7 +3665,7 @@
         <v>2011</v>
       </c>
       <c r="I34" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J34" t="s">
         <v>14</v>
@@ -3706,7 +3706,7 @@
         <v>2011</v>
       </c>
       <c r="I35" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J35" t="s">
         <v>14</v>
@@ -3791,7 +3791,7 @@
         <v>2012</v>
       </c>
       <c r="I37" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J37" t="s">
         <v>14</v>
@@ -3835,7 +3835,7 @@
         <v>2011</v>
       </c>
       <c r="I38" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J38" t="s">
         <v>14</v>
@@ -3958,7 +3958,7 @@
         <v>2011</v>
       </c>
       <c r="I41" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J41" t="s">
         <v>14</v>
@@ -4078,7 +4078,7 @@
         <v>2012</v>
       </c>
       <c r="I44" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J44" t="s">
         <v>14</v>
@@ -4119,7 +4119,7 @@
         <v>2015</v>
       </c>
       <c r="I45" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J45" t="s">
         <v>14</v>
@@ -4160,7 +4160,7 @@
         <v>2015</v>
       </c>
       <c r="I46" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J46" t="s">
         <v>14</v>
@@ -4201,7 +4201,7 @@
         <v>2012</v>
       </c>
       <c r="I47" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J47" t="s">
         <v>14</v>
@@ -4242,7 +4242,7 @@
         <v>2012</v>
       </c>
       <c r="I48" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J48" t="s">
         <v>14</v>
@@ -4283,7 +4283,7 @@
         <v>2015</v>
       </c>
       <c r="I49" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J49" t="s">
         <v>14</v>
@@ -4324,7 +4324,7 @@
         <v>2015</v>
       </c>
       <c r="I50" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J50" t="s">
         <v>14</v>
@@ -4365,7 +4365,7 @@
         <v>2012</v>
       </c>
       <c r="I51" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J51" t="s">
         <v>14</v>
@@ -4450,7 +4450,7 @@
         <v>2012</v>
       </c>
       <c r="I53" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J53" t="s">
         <v>14</v>
@@ -4491,7 +4491,7 @@
         <v>2012</v>
       </c>
       <c r="I54" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J54" t="s">
         <v>14</v>
@@ -4532,7 +4532,7 @@
         <v>2015</v>
       </c>
       <c r="I55" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J55" t="s">
         <v>14</v>
@@ -4573,7 +4573,7 @@
         <v>2015</v>
       </c>
       <c r="I56" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J56" t="s">
         <v>14</v>
@@ -4614,7 +4614,7 @@
         <v>2015</v>
       </c>
       <c r="I57" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J57" t="s">
         <v>14</v>
@@ -4655,7 +4655,7 @@
         <v>2012</v>
       </c>
       <c r="I58" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J58" t="s">
         <v>14</v>
@@ -4866,13 +4866,13 @@
         <v>34</v>
       </c>
       <c r="G63" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="H63">
         <v>2010</v>
       </c>
       <c r="I63" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="J63" t="s">
         <v>14</v>
@@ -4907,13 +4907,13 @@
         <v>34</v>
       </c>
       <c r="G64" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H64">
         <v>2017</v>
       </c>
       <c r="I64" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="J64" t="s">
         <v>14</v>
@@ -4948,7 +4948,7 @@
         <v>34</v>
       </c>
       <c r="G65" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H65">
         <v>2017</v>
@@ -4989,13 +4989,13 @@
         <v>34</v>
       </c>
       <c r="G66" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H66">
         <v>2018</v>
       </c>
       <c r="I66" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="J66" t="s">
         <v>14</v>
@@ -5030,7 +5030,7 @@
         <v>34</v>
       </c>
       <c r="G67" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="H67">
         <v>2017</v>
@@ -5147,7 +5147,7 @@
         <v>45</v>
       </c>
       <c r="G70" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="H70">
         <v>2008</v>
@@ -5188,7 +5188,7 @@
         <v>45</v>
       </c>
       <c r="G71" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="H71">
         <v>2013</v>
@@ -5270,10 +5270,10 @@
         <v>45</v>
       </c>
       <c r="G73" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I73" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="J73" t="s">
         <v>369</v>
@@ -5311,10 +5311,10 @@
         <v>45</v>
       </c>
       <c r="G74" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I74" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="J74" t="s">
         <v>369</v>
@@ -5399,7 +5399,7 @@
         <v>2006</v>
       </c>
       <c r="I76" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="J76" t="s">
         <v>14</v>
@@ -5434,7 +5434,7 @@
         <v>73</v>
       </c>
       <c r="G77" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="H77">
         <v>2010</v>
@@ -6096,7 +6096,7 @@
         <v>142</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="I93" t="s">
         <v>364</v>
@@ -6122,7 +6122,7 @@
         <v>13.95</v>
       </c>
       <c r="C94" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D94"/>
       <c r="E94" t="s">
@@ -6132,7 +6132,7 @@
         <v>147</v>
       </c>
       <c r="G94" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="H94"/>
       <c r="I94" t="s">
@@ -6207,7 +6207,7 @@
         <v>15.02</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1" t="s">
@@ -6338,7 +6338,7 @@
         <v>152</v>
       </c>
       <c r="G99" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I99" t="s">
         <v>402</v>
@@ -6376,7 +6376,7 @@
         <v>152</v>
       </c>
       <c r="G100" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I100" t="s">
         <v>402</v>
@@ -6415,7 +6415,7 @@
         <v>152</v>
       </c>
       <c r="G101" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="H101" s="1"/>
       <c r="I101" s="1" t="s">
@@ -6457,7 +6457,7 @@
         <v>152</v>
       </c>
       <c r="G102" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I102" t="s">
         <v>402</v>
@@ -6495,7 +6495,7 @@
         <v>152</v>
       </c>
       <c r="G103" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I103" t="s">
         <v>397</v>
@@ -6536,7 +6536,7 @@
         <v>152</v>
       </c>
       <c r="G104" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I104" t="s">
         <v>402</v>
@@ -6575,7 +6575,7 @@
         <v>152</v>
       </c>
       <c r="G105" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="H105"/>
       <c r="I105" t="s">
@@ -6615,7 +6615,7 @@
         <v>152</v>
       </c>
       <c r="G106" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="I106" t="s">
         <v>402</v>
@@ -6699,7 +6699,7 @@
         <v>195</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1" t="s">
@@ -6741,7 +6741,7 @@
         <v>195</v>
       </c>
       <c r="G109" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="H109">
         <v>1999</v>
@@ -6826,7 +6826,7 @@
         <v>197</v>
       </c>
       <c r="I111" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="J111" t="s">
         <v>369</v>
@@ -6993,7 +6993,7 @@
         <v>1994</v>
       </c>
       <c r="I115" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="J115" t="s">
         <v>14</v>
@@ -7028,7 +7028,7 @@
         <v>195</v>
       </c>
       <c r="G116" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="I116" t="s">
         <v>407</v>
@@ -7066,7 +7066,7 @@
         <v>195</v>
       </c>
       <c r="G117" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="I117" t="s">
         <v>408</v>
@@ -7148,7 +7148,7 @@
         <v>195</v>
       </c>
       <c r="G119" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="I119" t="s">
         <v>364</v>
@@ -7228,7 +7228,7 @@
         <v>195</v>
       </c>
       <c r="G121" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="H121">
         <v>1999</v>
@@ -7270,7 +7270,7 @@
         <v>195</v>
       </c>
       <c r="G122" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="H122">
         <v>1999</v>
@@ -7391,7 +7391,7 @@
         <v>195</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="H125" s="1">
         <v>2015</v>
@@ -7433,7 +7433,7 @@
         <v>195</v>
       </c>
       <c r="G126" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="H126" s="1">
         <v>2000</v>
@@ -7638,7 +7638,7 @@
         <v>133</v>
       </c>
       <c r="I131" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="J131" t="s">
         <v>366</v>
@@ -7857,7 +7857,7 @@
         <v>-81.623000000000005</v>
       </c>
       <c r="C137" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E137" t="s">
         <v>374</v>
@@ -7872,10 +7872,10 @@
         <v>2012</v>
       </c>
       <c r="I137" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="J137" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="K137" t="s">
         <v>15</v>
@@ -7913,7 +7913,7 @@
         <v>2013</v>
       </c>
       <c r="I138" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="J138" t="s">
         <v>311</v>
@@ -7957,7 +7957,7 @@
         <v>2013</v>
       </c>
       <c r="I139" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="J139" t="s">
         <v>311</v>
@@ -8001,7 +8001,7 @@
         <v>2015</v>
       </c>
       <c r="I140" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="J140" t="s">
         <v>311</v>
@@ -8030,7 +8030,7 @@
         <v>-92.22</v>
       </c>
       <c r="C141" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E141" t="s">
         <v>374</v>
@@ -8045,7 +8045,7 @@
         <v>2019</v>
       </c>
       <c r="I141" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="J141" t="s">
         <v>365</v>
@@ -8133,7 +8133,7 @@
         <v>2016</v>
       </c>
       <c r="I143" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="J143" t="s">
         <v>368</v>
@@ -8162,7 +8162,7 @@
         <v>-122.76</v>
       </c>
       <c r="C144" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E144" t="s">
         <v>374</v>
@@ -8221,7 +8221,7 @@
         <v>2011</v>
       </c>
       <c r="I145" t="s">
-        <v>469</v>
+        <v>611</v>
       </c>
       <c r="J145" t="s">
         <v>218</v>
@@ -8338,7 +8338,7 @@
         <v>-73.28</v>
       </c>
       <c r="C148" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="E148" t="s">
         <v>374</v>
@@ -8379,7 +8379,7 @@
         <v>-72.11</v>
       </c>
       <c r="C149" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D149" t="s">
         <v>261</v>
@@ -8423,7 +8423,7 @@
         <v>-72.8</v>
       </c>
       <c r="C150" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E150" t="s">
         <v>374</v>
@@ -8464,7 +8464,7 @@
         <v>-71.86</v>
       </c>
       <c r="C151" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D151" t="s">
         <v>262</v>
@@ -8508,7 +8508,7 @@
         <v>-72.38</v>
       </c>
       <c r="C152" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E152" t="s">
         <v>374</v>
@@ -8549,7 +8549,7 @@
         <v>-72.180000000000007</v>
       </c>
       <c r="C153" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D153" t="s">
         <v>263</v>
@@ -8593,7 +8593,7 @@
         <v>-75.430000000000007</v>
       </c>
       <c r="C154" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E154" t="s">
         <v>374</v>
@@ -8816,7 +8816,7 @@
         <v>58</v>
       </c>
       <c r="I159" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="J159" t="s">
         <v>308</v>
@@ -8845,7 +8845,7 @@
         <v>-84.23</v>
       </c>
       <c r="C160" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E160" t="s">
         <v>374</v>
@@ -8939,7 +8939,7 @@
         <v>58</v>
       </c>
       <c r="I162" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="J162" t="s">
         <v>308</v>
@@ -9012,7 +9012,7 @@
         <v>-89.37</v>
       </c>
       <c r="C164" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D164" t="s">
         <v>236</v>
@@ -9059,7 +9059,7 @@
         <v>-87.7</v>
       </c>
       <c r="C165" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E165" t="s">
         <v>374</v>
@@ -9100,7 +9100,7 @@
         <v>-87.85</v>
       </c>
       <c r="C166" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D166" t="s">
         <v>238</v>
@@ -9162,7 +9162,7 @@
         <v>2015</v>
       </c>
       <c r="I167" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="J167" t="s">
         <v>369</v>
@@ -9191,7 +9191,7 @@
         <v>-84.51</v>
       </c>
       <c r="C168" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D168" t="s">
         <v>343</v>
@@ -9235,7 +9235,7 @@
         <v>-84.88</v>
       </c>
       <c r="C169" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="E169" t="s">
         <v>374</v>
@@ -9273,7 +9273,7 @@
         <v>-85.64</v>
       </c>
       <c r="C170" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E170" t="s">
         <v>374</v>
@@ -9311,7 +9311,7 @@
         <v>-84.65</v>
       </c>
       <c r="C171" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E171" t="s">
         <v>374</v>
@@ -9349,7 +9349,7 @@
         <v>-86.22</v>
       </c>
       <c r="C172" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E172" t="s">
         <v>374</v>
@@ -9387,7 +9387,7 @@
         <v>-85.48</v>
       </c>
       <c r="C173" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E173" t="s">
         <v>374</v>
@@ -9478,7 +9478,7 @@
         <v>2014</v>
       </c>
       <c r="I175" t="s">
-        <v>470</v>
+        <v>612</v>
       </c>
       <c r="J175" t="s">
         <v>218</v>
@@ -9507,7 +9507,7 @@
         <v>-76.849999999999994</v>
       </c>
       <c r="C176" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D176" t="s">
         <v>241</v>
@@ -9554,7 +9554,7 @@
         <v>-75.430000000000007</v>
       </c>
       <c r="C177" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E177" t="s">
         <v>374</v>
@@ -9595,7 +9595,7 @@
         <v>-70.27</v>
       </c>
       <c r="C178" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D178" t="s">
         <v>239</v>
@@ -9639,7 +9639,7 @@
         <v>-71.290000000000006</v>
       </c>
       <c r="C179" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E179" t="s">
         <v>374</v>
@@ -9680,7 +9680,7 @@
         <v>-70.72</v>
       </c>
       <c r="C180" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E180" t="s">
         <v>374</v>
@@ -9721,7 +9721,7 @@
         <v>-85.36</v>
       </c>
       <c r="C181" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E181" t="s">
         <v>374</v>
@@ -9762,7 +9762,7 @@
         <v>-83.34</v>
       </c>
       <c r="C182" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E182" t="s">
         <v>374</v>
@@ -9803,7 +9803,7 @@
         <v>-86.09</v>
       </c>
       <c r="C183" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E183" t="s">
         <v>374</v>
@@ -9844,7 +9844,7 @@
         <v>-83.85</v>
       </c>
       <c r="C184" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E184" t="s">
         <v>374</v>
@@ -9885,7 +9885,7 @@
         <v>-74.099999999999994</v>
       </c>
       <c r="C185" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E185" t="s">
         <v>374</v>
@@ -10011,7 +10011,7 @@
         <v>-75.06</v>
       </c>
       <c r="C188" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E188" t="s">
         <v>374</v>
@@ -10184,7 +10184,7 @@
         <v>-74.64</v>
       </c>
       <c r="C192" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E192" t="s">
         <v>374</v>
@@ -10307,7 +10307,7 @@
         <v>-73.56</v>
       </c>
       <c r="C195" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E195" t="s">
         <v>374</v>
@@ -10322,7 +10322,7 @@
         <v>2011</v>
       </c>
       <c r="I195" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="J195" t="s">
         <v>367</v>
@@ -10389,7 +10389,7 @@
         <v>-73.56</v>
       </c>
       <c r="C197" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E197" t="s">
         <v>374</v>
@@ -10404,7 +10404,7 @@
         <v>2018</v>
       </c>
       <c r="I197" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="J197" t="s">
         <v>369</v>
@@ -10433,7 +10433,7 @@
         <v>-72.62</v>
       </c>
       <c r="C198" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="E198" t="s">
         <v>374</v>
@@ -10474,7 +10474,7 @@
         <v>-73.77</v>
       </c>
       <c r="C199" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D199" t="s">
         <v>338</v>
@@ -10612,7 +10612,7 @@
         <v>2021</v>
       </c>
       <c r="I202" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="J202" t="s">
         <v>308</v>
@@ -10691,7 +10691,7 @@
         <v>2011</v>
       </c>
       <c r="I204" t="s">
-        <v>471</v>
+        <v>613</v>
       </c>
       <c r="J204" t="s">
         <v>218</v>
@@ -10843,7 +10843,7 @@
         <v>-83.68</v>
       </c>
       <c r="C208" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E208" t="s">
         <v>374</v>
@@ -10884,7 +10884,7 @@
         <v>-81.680000000000007</v>
       </c>
       <c r="C209" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E209" t="s">
         <v>374</v>
@@ -10925,7 +10925,7 @@
         <v>-82.99</v>
       </c>
       <c r="C210" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E210" t="s">
         <v>374</v>
@@ -10966,7 +10966,7 @@
         <v>-82.3</v>
       </c>
       <c r="C211" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E211" t="s">
         <v>374</v>
@@ -11007,7 +11007,7 @@
         <v>-81.290000000000006</v>
       </c>
       <c r="C212" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D212" t="s">
         <v>339</v>
@@ -11048,7 +11048,7 @@
         <v>-82.48</v>
       </c>
       <c r="C213" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E213" t="s">
         <v>374</v>
@@ -11151,7 +11151,7 @@
         <v>2014</v>
       </c>
       <c r="I215" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="K215" t="s">
         <v>25</v>
@@ -11368,7 +11368,7 @@
         <v>2014</v>
       </c>
       <c r="I220" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="K220" t="s">
         <v>25</v>
@@ -11482,7 +11482,7 @@
         <v>-78.38</v>
       </c>
       <c r="C223" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E223" t="s">
         <v>374</v>
@@ -11523,7 +11523,7 @@
         <v>-75.25</v>
       </c>
       <c r="C224" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E224" t="s">
         <v>374</v>
@@ -11561,7 +11561,7 @@
         <v>-75.67</v>
       </c>
       <c r="C225" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E225" t="s">
         <v>374</v>
@@ -11599,7 +11599,7 @@
         <v>-75.099999999999994</v>
       </c>
       <c r="C226" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E226" t="s">
         <v>374</v>
@@ -11643,7 +11643,7 @@
         <v>-76.36</v>
       </c>
       <c r="C227" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E227" t="s">
         <v>374</v>
@@ -11681,7 +11681,7 @@
         <v>-77.239999999999995</v>
       </c>
       <c r="C228" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E228" t="s">
         <v>374</v>
@@ -11725,7 +11725,7 @@
         <v>-79.11</v>
       </c>
       <c r="C229" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E229" t="s">
         <v>374</v>
@@ -11810,7 +11810,7 @@
         <v>-76.38</v>
       </c>
       <c r="C231" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D231" t="s">
         <v>340</v>
@@ -11898,7 +11898,7 @@
         <v>-76.180000000000007</v>
       </c>
       <c r="C233" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E233" t="s">
         <v>374</v>
@@ -11936,7 +11936,7 @@
         <v>-76.180000000000007</v>
       </c>
       <c r="C234" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E234" t="s">
         <v>374</v>
@@ -11974,7 +11974,7 @@
         <v>-71.77</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D235" s="1" t="s">
         <v>341</v>
@@ -12097,7 +12097,7 @@
         <v>-83.85</v>
       </c>
       <c r="C238" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E238" t="s">
         <v>374</v>
@@ -12138,7 +12138,7 @@
         <v>-84.86</v>
       </c>
       <c r="C239" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="E239" t="s">
         <v>374</v>
@@ -12179,7 +12179,7 @@
         <v>-86.05</v>
       </c>
       <c r="C240" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E240" t="s">
         <v>374</v>
@@ -12220,7 +12220,7 @@
         <v>-86.82</v>
       </c>
       <c r="C241" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E241" t="s">
         <v>374</v>
@@ -12261,7 +12261,7 @@
         <v>-86.98</v>
       </c>
       <c r="C242" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E242" t="s">
         <v>374</v>
@@ -12302,7 +12302,7 @@
         <v>-85.68</v>
       </c>
       <c r="C243" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E243" t="s">
         <v>374</v>
@@ -12343,7 +12343,7 @@
         <v>-85.15</v>
       </c>
       <c r="C244" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E244" t="s">
         <v>374</v>
@@ -12384,7 +12384,7 @@
         <v>-83.94</v>
       </c>
       <c r="C245" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E245" t="s">
         <v>374</v>
@@ -12425,7 +12425,7 @@
         <v>-86.34</v>
       </c>
       <c r="C246" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E246" t="s">
         <v>374</v>
@@ -12466,7 +12466,7 @@
         <v>-86.86</v>
       </c>
       <c r="C247" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="E247" t="s">
         <v>374</v>
@@ -12507,7 +12507,7 @@
         <v>-78.61</v>
       </c>
       <c r="C248" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E248" t="s">
         <v>374</v>
@@ -12548,7 +12548,7 @@
         <v>-79.11</v>
       </c>
       <c r="C249" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E249" t="s">
         <v>374</v>
@@ -12589,7 +12589,7 @@
         <v>-79.25</v>
       </c>
       <c r="C250" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E250" t="s">
         <v>374</v>
@@ -12630,7 +12630,7 @@
         <v>-79.47</v>
       </c>
       <c r="C251" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E251" t="s">
         <v>374</v>
@@ -12671,7 +12671,7 @@
         <v>-80.72</v>
       </c>
       <c r="C252" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E252" t="s">
         <v>374</v>
@@ -12724,7 +12724,7 @@
         <v>245</v>
       </c>
       <c r="I253" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="J253" t="s">
         <v>311</v>
@@ -12753,7 +12753,7 @@
         <v>-77.61</v>
       </c>
       <c r="C254" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E254" t="s">
         <v>374</v>
@@ -12768,7 +12768,7 @@
         <v>2013</v>
       </c>
       <c r="I254" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="J254" t="s">
         <v>369</v>
@@ -12797,7 +12797,7 @@
         <v>-77.97</v>
       </c>
       <c r="C255" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E255" t="s">
         <v>374</v>
@@ -12838,7 +12838,7 @@
         <v>-76.959999999999994</v>
       </c>
       <c r="C256" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="E256" t="s">
         <v>374</v>
@@ -12879,7 +12879,7 @@
         <v>-77.239999999999995</v>
       </c>
       <c r="C257" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E257" t="s">
         <v>374</v>
@@ -12920,7 +12920,7 @@
         <v>-77.790000000000006</v>
       </c>
       <c r="C258" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E258" t="s">
         <v>374</v>
@@ -12961,7 +12961,7 @@
         <v>-80.319999999999993</v>
       </c>
       <c r="C259" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E259" t="s">
         <v>374</v>
@@ -13002,7 +13002,7 @@
         <v>-81.209999999999994</v>
       </c>
       <c r="C260" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E260" t="s">
         <v>374</v>
@@ -13043,7 +13043,7 @@
         <v>-78.930000000000007</v>
       </c>
       <c r="C261" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E261" t="s">
         <v>374</v>
@@ -13084,7 +13084,7 @@
         <v>-77.52</v>
       </c>
       <c r="C262" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E262" t="s">
         <v>374</v>
@@ -13125,7 +13125,7 @@
         <v>-77.33</v>
       </c>
       <c r="C263" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E263" t="s">
         <v>374</v>
@@ -13166,7 +13166,7 @@
         <v>-79.959999999999994</v>
       </c>
       <c r="C264" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E264" t="s">
         <v>374</v>
@@ -13207,7 +13207,7 @@
         <v>-76.8</v>
       </c>
       <c r="C265" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E265" t="s">
         <v>374</v>
@@ -13248,7 +13248,7 @@
         <v>-77.650000000000006</v>
       </c>
       <c r="C266" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E266" t="s">
         <v>374</v>
@@ -13289,7 +13289,7 @@
         <v>-77.97</v>
       </c>
       <c r="C267" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E267" t="s">
         <v>374</v>
@@ -13342,7 +13342,7 @@
         <v>245</v>
       </c>
       <c r="I268" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="J268" t="s">
         <v>311</v>
@@ -13412,7 +13412,7 @@
         <v>-76.290000000000006</v>
       </c>
       <c r="C270" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="E270" t="s">
         <v>374</v>
@@ -13453,7 +13453,7 @@
         <v>-75.900000000000006</v>
       </c>
       <c r="C271" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E271" t="s">
         <v>374</v>
@@ -13494,7 +13494,7 @@
         <v>-79.47</v>
       </c>
       <c r="C272" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E272" t="s">
         <v>374</v>
@@ -13535,7 +13535,7 @@
         <v>-77.88</v>
       </c>
       <c r="C273" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E273" t="s">
         <v>374</v>
@@ -13576,7 +13576,7 @@
         <v>-78.430000000000007</v>
       </c>
       <c r="C274" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E274" t="s">
         <v>374</v>
@@ -13617,7 +13617,7 @@
         <v>-77.61</v>
       </c>
       <c r="C275" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E275" t="s">
         <v>374</v>
@@ -13699,7 +13699,7 @@
         <v>-80.12</v>
       </c>
       <c r="C277" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E277" t="s">
         <v>374</v>
@@ -13740,7 +13740,7 @@
         <v>-78.88</v>
       </c>
       <c r="C278" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E278" t="s">
         <v>374</v>
@@ -13781,7 +13781,7 @@
         <v>-78.63</v>
       </c>
       <c r="C279" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E279" t="s">
         <v>374</v>
@@ -13822,7 +13822,7 @@
         <v>-77.61</v>
       </c>
       <c r="C280" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E280" t="s">
         <v>374</v>
@@ -13863,7 +13863,7 @@
         <v>-77.42</v>
       </c>
       <c r="C281" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E281" t="s">
         <v>374</v>
@@ -13989,7 +13989,7 @@
         <v>-81.95</v>
       </c>
       <c r="C284" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E284" t="s">
         <v>374</v>
@@ -14030,7 +14030,7 @@
         <v>-76.78</v>
       </c>
       <c r="C285" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E285" t="s">
         <v>374</v>
@@ -14115,7 +14115,7 @@
         <v>-81.08</v>
       </c>
       <c r="C287" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="E287" t="s">
         <v>374</v>
@@ -14156,7 +14156,7 @@
         <v>-76.53</v>
       </c>
       <c r="C288" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E288" t="s">
         <v>374</v>
@@ -14241,7 +14241,7 @@
         <v>-89.55</v>
       </c>
       <c r="C290" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E290" t="s">
         <v>374</v>
@@ -14256,7 +14256,7 @@
         <v>2019</v>
       </c>
       <c r="I290" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="J290" t="s">
         <v>369</v>
@@ -14285,7 +14285,7 @@
         <v>-87.84</v>
       </c>
       <c r="C291" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="D291" t="s">
         <v>287</v>
@@ -14303,7 +14303,7 @@
         <v>448</v>
       </c>
       <c r="I291" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J291" t="s">
         <v>365</v>
@@ -14332,7 +14332,7 @@
         <v>-87.91</v>
       </c>
       <c r="C292" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E292" t="s">
         <v>374</v>
@@ -14347,7 +14347,7 @@
         <v>448</v>
       </c>
       <c r="I292" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J292" t="s">
         <v>27</v>
@@ -14376,7 +14376,7 @@
         <v>-87.62</v>
       </c>
       <c r="C293" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E293" t="s">
         <v>374</v>
@@ -14391,7 +14391,7 @@
         <v>448</v>
       </c>
       <c r="I293" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J293" t="s">
         <v>27</v>

</xml_diff>